<commit_message>
resized imgs (not centered)
</commit_message>
<xml_diff>
--- a/dataset_with_images.xlsx
+++ b/dataset_with_images.xlsx
@@ -133,7 +133,7 @@
       <row>1</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="6858000" cy="5143500"/>
+    <ext cx="4876800" cy="4876800"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -158,7 +158,7 @@
       <row>2</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="14630400" cy="19507200"/>
+    <ext cx="4876800" cy="4876800"/>
     <pic>
       <nvPicPr>
         <cNvPr id="2" name="Image 2" descr="Picture"/>
@@ -183,7 +183,7 @@
       <row>3</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="3676650" cy="6667500"/>
+    <ext cx="4876800" cy="4876800"/>
     <pic>
       <nvPicPr>
         <cNvPr id="3" name="Image 3" descr="Picture"/>
@@ -208,7 +208,7 @@
       <row>4</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="4848225" cy="6191250"/>
+    <ext cx="4876800" cy="4876800"/>
     <pic>
       <nvPicPr>
         <cNvPr id="4" name="Image 4" descr="Picture"/>
@@ -233,7 +233,7 @@
       <row>5</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="9144000" cy="10287000"/>
+    <ext cx="4876800" cy="4876800"/>
     <pic>
       <nvPicPr>
         <cNvPr id="5" name="Image 5" descr="Picture"/>
@@ -258,7 +258,7 @@
       <row>6</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="14287500" cy="8039100"/>
+    <ext cx="4876800" cy="4876800"/>
     <pic>
       <nvPicPr>
         <cNvPr id="6" name="Image 6" descr="Picture"/>
@@ -283,7 +283,7 @@
       <row>7</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8496300" cy="6448425"/>
+    <ext cx="4876800" cy="4876800"/>
     <pic>
       <nvPicPr>
         <cNvPr id="7" name="Image 7" descr="Picture"/>
@@ -308,7 +308,7 @@
       <row>8</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8801100" cy="4943475"/>
+    <ext cx="4876800" cy="4876800"/>
     <pic>
       <nvPicPr>
         <cNvPr id="8" name="Image 8" descr="Picture"/>
@@ -333,7 +333,7 @@
       <row>9</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="18192750" cy="9525000"/>
+    <ext cx="4876800" cy="4876800"/>
     <pic>
       <nvPicPr>
         <cNvPr id="9" name="Image 9" descr="Picture"/>
@@ -358,7 +358,7 @@
       <row>10</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="15240000" cy="11020425"/>
+    <ext cx="4876800" cy="4876800"/>
     <pic>
       <nvPicPr>
         <cNvPr id="10" name="Image 10" descr="Picture"/>
@@ -383,7 +383,7 @@
       <row>14</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="18830925" cy="16354425"/>
+    <ext cx="4876800" cy="4876800"/>
     <pic>
       <nvPicPr>
         <cNvPr id="11" name="Image 11" descr="Picture"/>
@@ -408,7 +408,7 @@
       <row>15</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="4562475" cy="5581650"/>
+    <ext cx="4876800" cy="4876800"/>
     <pic>
       <nvPicPr>
         <cNvPr id="12" name="Image 12" descr="Picture"/>
@@ -433,7 +433,7 @@
       <row>16</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="6810375" cy="3829050"/>
+    <ext cx="4876800" cy="4876800"/>
     <pic>
       <nvPicPr>
         <cNvPr id="13" name="Image 13" descr="Picture"/>

</xml_diff>